<commit_message>
Completed Influence and Timer Backend. (0.6-D1)
</commit_message>
<xml_diff>
--- a/Influence Rate Calculations.xlsx
+++ b/Influence Rate Calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="27795" windowHeight="11310"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="27795" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
   <si>
     <t>4 Owned</t>
   </si>
@@ -52,14 +52,66 @@
   </si>
   <si>
     <t>Diff.</t>
+  </si>
+  <si>
+    <t>Float Value</t>
+  </si>
+  <si>
+    <t>Short Value</t>
+  </si>
+  <si>
+    <t>Anim Rate</t>
+  </si>
+  <si>
+    <t>Percentage Required</t>
+  </si>
+  <si>
+    <t>1 Owned</t>
+  </si>
+  <si>
+    <t>1% +</t>
+  </si>
+  <si>
+    <t>4 Flag Base</t>
+  </si>
+  <si>
+    <t>3 Flag Base</t>
+  </si>
+  <si>
+    <t>2 Flag Base</t>
+  </si>
+  <si>
+    <t>1 Flag Base</t>
+  </si>
+  <si>
+    <t>66% +</t>
+  </si>
+  <si>
+    <t>33% +</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,15 +139,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,169 +457,561 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2-E2</f>
-        <v>1</v>
-      </c>
-      <c r="G2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <f>D3-E3</f>
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" ref="F3:F7" si="0">D3-E3</f>
-        <v>0.75</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2">
         <v>0.75</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:F8" si="0">D4-E4</f>
+        <v>0.75</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E5" s="2">
         <v>0.25</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F5" s="2">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D6" s="2">
         <v>0.5</v>
       </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D7" s="2">
         <v>0.5</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E7" s="2">
         <v>0.25</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F7" s="2">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D8" s="2">
         <v>0.5</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E8" s="2">
         <v>0.5</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <f>D12-E12</f>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" ref="F13:F14" si="1">D13-E13</f>
+        <v>0.66</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.33</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" ref="F19" si="2">D19-E19</f>
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <f>D20-E20</f>
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="2">
+        <f>D21-E21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" ref="F25" si="3">D25-E25</f>
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>2.35</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>1.55</v>
+      </c>
+      <c r="C30">
+        <v>60</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C31">
+        <v>80</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>0.92</v>
+      </c>
+      <c r="C32">
+        <v>100</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+  <mergeCells count="8">
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A17:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>